<commit_message>
arrumei o arquivo modelo de importação de transações
</commit_message>
<xml_diff>
--- a/server/public/modelo-transacoes.xlsx
+++ b/server/public/modelo-transacoes.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -421,58 +421,211 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>2025-09-23</v>
+        <v>2024-09-01</v>
       </c>
       <c r="B2" t="str">
-        <v>Venda de produto A</v>
+        <v>Venda de produtos no varejo</v>
       </c>
       <c r="C2">
-        <v>150</v>
+        <v>1250</v>
       </c>
       <c r="D2" t="str">
-        <v>Entrada</v>
+        <v>Receita</v>
       </c>
       <c r="E2" t="str">
-        <v>Vendas</v>
+        <v>Varejo</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>2025-09-23</v>
+        <v>2024-09-02</v>
       </c>
       <c r="B3" t="str">
-        <v>Compra de material</v>
+        <v>Venda em atacado para distribuidor</v>
       </c>
       <c r="C3">
-        <v>75.5</v>
+        <v>3500</v>
       </c>
       <c r="D3" t="str">
-        <v>Saída</v>
+        <v>Receita</v>
       </c>
       <c r="E3" t="str">
-        <v>Compras</v>
+        <v>Atacado</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>2025-09-23</v>
+        <v>2024-09-03</v>
       </c>
       <c r="B4" t="str">
-        <v>Pagamento de serviço</v>
+        <v>Rendimento de investimentos</v>
       </c>
       <c r="C4">
-        <v>200</v>
+        <v>450</v>
       </c>
       <c r="D4" t="str">
-        <v>Saída</v>
+        <v>Receita</v>
       </c>
       <c r="E4" t="str">
-        <v>Serviços</v>
+        <v>Investimentos</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>2024-09-04</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Serviços de consultoria</v>
+      </c>
+      <c r="C5">
+        <v>800</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Receita</v>
+      </c>
+      <c r="E5" t="str">
+        <v>Outros</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>2024-09-05</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Venda online de produtos</v>
+      </c>
+      <c r="C6">
+        <v>680</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Receita</v>
+      </c>
+      <c r="E6" t="str">
+        <v>Varejo</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>2024-09-01</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Aluguel do escritório</v>
+      </c>
+      <c r="C7">
+        <v>1200</v>
+      </c>
+      <c r="D7" t="str">
+        <v>Despesa</v>
+      </c>
+      <c r="E7" t="str">
+        <v>Fixo</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>2024-09-02</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Compra de matéria-prima</v>
+      </c>
+      <c r="C8">
+        <v>850</v>
+      </c>
+      <c r="D8" t="str">
+        <v>Despesa</v>
+      </c>
+      <c r="E8" t="str">
+        <v>Variável</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>2024-09-03</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Compra de equipamentos</v>
+      </c>
+      <c r="C9">
+        <v>2500</v>
+      </c>
+      <c r="D9" t="str">
+        <v>Despesa</v>
+      </c>
+      <c r="E9" t="str">
+        <v>Investimento</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>2024-09-04</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Campanha de marketing digital</v>
+      </c>
+      <c r="C10">
+        <v>300</v>
+      </c>
+      <c r="D10" t="str">
+        <v>Despesa</v>
+      </c>
+      <c r="E10" t="str">
+        <v>Mkt</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>2024-09-05</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Despesas administrativas</v>
+      </c>
+      <c r="C11">
+        <v>150</v>
+      </c>
+      <c r="D11" t="str">
+        <v>Despesa</v>
+      </c>
+      <c r="E11" t="str">
+        <v>Outros</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>2024-09-06</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Salários dos funcionários</v>
+      </c>
+      <c r="C12">
+        <v>3200</v>
+      </c>
+      <c r="D12" t="str">
+        <v>Despesa</v>
+      </c>
+      <c r="E12" t="str">
+        <v>Fixo</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>2024-09-07</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Combustível para entrega</v>
+      </c>
+      <c r="C13">
+        <v>180</v>
+      </c>
+      <c r="D13" t="str">
+        <v>Despesa</v>
+      </c>
+      <c r="E13" t="str">
+        <v>Variável</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E13"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>